<commit_message>
corrected column from biosampleNumber to bioSampleNumber
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_H.BROWN_08.21.20.xlsx
+++ b/bioSample/bioSample_H.BROWN_08.21.20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5501BD1D-8524-3141-BF97-9B5BB92EAC5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34F09A8-9780-0149-A6C1-C36574BC67FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{CA705446-5DD0-5A4B-9B22-AD6ADC21E26B}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>harvester</t>
   </si>
   <si>
-    <t>biosampleNumber</t>
-  </si>
-  <si>
     <t>experimentDesign</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>CNAG_03894</t>
+  </si>
+  <si>
+    <t>bioSampleNumber</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -446,48 +446,48 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
       <c r="H2">
         <v>1440</v>
@@ -498,25 +498,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
       </c>
       <c r="H3">
         <v>1440</v>
@@ -527,25 +527,25 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
         <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
       </c>
       <c r="H4">
         <v>1440</v>
@@ -556,25 +556,25 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
         <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
       </c>
       <c r="H5">
         <v>1440</v>
@@ -585,25 +585,25 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6">
         <v>1440</v>
@@ -614,25 +614,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>16</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7">
         <v>1440</v>
@@ -643,25 +643,25 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8">
         <v>1440</v>
@@ -672,25 +672,25 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9">
         <v>1440</v>

</xml_diff>